<commit_message>
Novos casos de testes
Inclusão do Enum para o código de erro e criação dos casos de teste
inválidos do comprimento e peso.
</commit_message>
<xml_diff>
--- a/TabelaDecisao.xlsx
+++ b/TabelaDecisao.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc3f68fe0d6ed5e6/INF321 Verificação ^0 Validação/Lab03/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20376" windowHeight="9048"/>
   </bookViews>
   <sheets>
     <sheet name="UC01" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="62">
   <si>
     <t>peso</t>
   </si>
@@ -59,9 +54,6 @@
     <t>&gt;0</t>
   </si>
   <si>
-    <t>&lt;=0</t>
-  </si>
-  <si>
     <t>CEP Valido</t>
   </si>
   <si>
@@ -183,13 +175,43 @@
   </si>
   <si>
     <t>&gt;15 e &lt;=30</t>
+  </si>
+  <si>
+    <t>&lt;16</t>
+  </si>
+  <si>
+    <t>&gt;= 16 e &lt;=105</t>
+  </si>
+  <si>
+    <t>&gt; 105</t>
+  </si>
+  <si>
+    <t>&gt;=11 e &lt;= 105</t>
+  </si>
+  <si>
+    <t>&lt; 11</t>
+  </si>
+  <si>
+    <t>&gt;=2 e &lt;=105</t>
+  </si>
+  <si>
+    <t>&lt; 2</t>
+  </si>
+  <si>
+    <t>largura+altura+comprimento</t>
+  </si>
+  <si>
+    <t>&lt;= 200</t>
+  </si>
+  <si>
+    <t>&gt; 200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,22 +266,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thick">
@@ -281,8 +317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A2:O16" totalsRowShown="0" tableBorderDxfId="0">
-  <autoFilter ref="A2:O16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A2:O21" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A2:O21"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Entrada"/>
     <tableColumn id="2" name="Condições"/>
@@ -292,7 +328,7 @@
     <tableColumn id="6" name="T4"/>
     <tableColumn id="7" name="T5"/>
     <tableColumn id="8" name="T6"/>
-    <tableColumn id="9" name="T7"/>
+    <tableColumn id="9" name="T7" dataDxfId="0"/>
     <tableColumn id="10" name="T8"/>
     <tableColumn id="11" name="T9"/>
     <tableColumn id="12" name="T10"/>
@@ -305,8 +341,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A17:O20" totalsRowShown="0">
-  <autoFilter ref="A17:O20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A22:O25" totalsRowShown="0">
+  <autoFilter ref="A22:O25"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Saida"/>
     <tableColumn id="2" name="Ações"/>
@@ -371,7 +407,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,7 +442,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,99 +619,99 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C16" sqref="C16:I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="15" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="15" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" ht="19.8">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>33</v>
       </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -683,13 +719,28 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -697,13 +748,28 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -711,13 +777,28 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -725,13 +806,28 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
+      <c r="B7" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -739,214 +835,558 @@
       <c r="D7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22" t="s">
+        <v>44</v>
+      </c>
+      <c r="N22" t="s">
+        <v>45</v>
+      </c>
+      <c r="O22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" t="s">
-        <v>44</v>
-      </c>
-      <c r="M17" t="s">
-        <v>45</v>
-      </c>
-      <c r="N17" t="s">
-        <v>46</v>
-      </c>
-      <c r="O17" t="s">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
+      <c r="D25" s="5">
+        <v>-21</v>
+      </c>
+      <c r="E25" s="5">
+        <v>-4</v>
+      </c>
+      <c r="F25" s="5">
+        <v>-4</v>
+      </c>
+      <c r="G25" s="5">
+        <v>-4</v>
+      </c>
+      <c r="H25">
+        <v>-22</v>
+      </c>
+      <c r="I25" s="5">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="C26" s="1"/>
+      <c r="E26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Padronizado Nome de Testes + 4 novos testes
</commit_message>
<xml_diff>
--- a/TabelaDecisao.xlsx
+++ b/TabelaDecisao.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\INF321_LAB_TDD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20376" windowHeight="9048"/>
+    <workbookView xWindow="5130" yWindow="0" windowWidth="20370" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="UC01" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="64">
   <si>
     <t>peso</t>
   </si>
@@ -205,13 +210,19 @@
   </si>
   <si>
     <t>&gt; 200</t>
+  </si>
+  <si>
+    <t>!=(41106, 40010, 40215, 40045, 40290)</t>
+  </si>
+  <si>
+    <t>=(40045,40290)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +244,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -266,17 +283,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A2:O21" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A2:O21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A2:O23" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A2:O23"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Entrada"/>
     <tableColumn id="2" name="Condições"/>
@@ -341,8 +359,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A22:O25" totalsRowShown="0">
-  <autoFilter ref="A22:O25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A24:O27" totalsRowShown="0">
+  <autoFilter ref="A24:O27"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Saida"/>
     <tableColumn id="2" name="Ações"/>
@@ -619,47 +637,50 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:I16"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="15" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.8">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -706,7 +727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -731,11 +752,23 @@
       <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -760,11 +793,23 @@
       <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="I4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -789,11 +834,23 @@
       <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="I5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -815,18 +872,30 @@
       <c r="G6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="H6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C7" t="s">
@@ -850,8 +919,20 @@
       <c r="I7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -879,8 +960,20 @@
       <c r="I8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -905,11 +998,23 @@
       <c r="H9" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="I9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -934,40 +1039,64 @@
       <c r="H10" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="I10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -992,11 +1121,23 @@
       <c r="H12" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="I12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1021,40 +1162,64 @@
       <c r="H13" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="I13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1082,37 +1247,61 @@
       <c r="I15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="C16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1137,11 +1326,23 @@
       <c r="H17" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="I17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1166,11 +1367,23 @@
       <c r="H18" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="I18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1195,198 +1408,352 @@
       <c r="H19" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="I19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" t="s">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" t="s">
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F24" t="s">
         <v>37</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G24" t="s">
         <v>38</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H24" t="s">
         <v>39</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I24" t="s">
         <v>40</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J24" t="s">
         <v>41</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K24" t="s">
         <v>42</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L24" t="s">
         <v>43</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M24" t="s">
         <v>44</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N24" t="s">
         <v>45</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
-      <c r="A23" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>10</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" t="s">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D27" s="4">
         <v>-21</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E27" s="3">
         <v>-4</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F27" s="4">
         <v>-4</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G27" s="4">
         <v>-4</v>
       </c>
-      <c r="H25">
+      <c r="H27">
         <v>-22</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I27" s="4">
         <v>-15</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="C26" s="1"/>
-      <c r="E26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="J27">
+        <v>-1</v>
+      </c>
+      <c r="K27">
+        <v>-3</v>
+      </c>
+      <c r="L27">
+        <v>-16</v>
+      </c>
+      <c r="M27">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="E28" s="3"/>
+      <c r="H28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Novos teste e stub (wiremock)
Inclusção do stub wiremock, para realizar os casos de testes do UC02 e
novos testes do UC01.
</commit_message>
<xml_diff>
--- a/TabelaDecisao.xlsx
+++ b/TabelaDecisao.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\INF321_LAB_TDD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="0" windowWidth="20370" windowHeight="9045"/>
+    <workbookView xWindow="5136" yWindow="0" windowWidth="20376" windowHeight="9048"/>
   </bookViews>
   <sheets>
     <sheet name="UC01" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="68">
   <si>
     <t>peso</t>
   </si>
@@ -216,13 +211,25 @@
   </si>
   <si>
     <t>=(40045,40290)</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>R15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,10 +298,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,9 +342,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A2:O23" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A2:O23"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A2:Q23" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A2:Q23">
+    <filterColumn colId="15"/>
+    <filterColumn colId="16"/>
+  </autoFilter>
+  <tableColumns count="17">
     <tableColumn id="1" name="Entrada"/>
     <tableColumn id="2" name="Condições"/>
     <tableColumn id="3" name="T1"/>
@@ -353,15 +363,20 @@
     <tableColumn id="13" name="T11"/>
     <tableColumn id="14" name="T12"/>
     <tableColumn id="15" name="T13"/>
+    <tableColumn id="16" name="T14"/>
+    <tableColumn id="17" name="T15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A24:O27" totalsRowShown="0">
-  <autoFilter ref="A24:O27"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A24:Q27" totalsRowShown="0">
+  <autoFilter ref="A24:Q27">
+    <filterColumn colId="15"/>
+    <filterColumn colId="16"/>
+  </autoFilter>
+  <tableColumns count="17">
     <tableColumn id="1" name="Saida"/>
     <tableColumn id="2" name="Ações"/>
     <tableColumn id="3" name="R1"/>
@@ -377,6 +392,8 @@
     <tableColumn id="13" name="R11"/>
     <tableColumn id="14" name="R12"/>
     <tableColumn id="15" name="R13"/>
+    <tableColumn id="17" name="R14"/>
+    <tableColumn id="18" name="R15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -637,50 +654,50 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="15" width="6.7109375" customWidth="1"/>
+    <col min="3" max="15" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" ht="19.8">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -726,8 +743,14 @@
       <c r="O2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -767,8 +790,20 @@
       <c r="M3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -808,8 +843,20 @@
       <c r="M4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -849,8 +896,20 @@
       <c r="M5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -890,8 +949,20 @@
       <c r="M6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -931,8 +1002,20 @@
       <c r="M7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -972,8 +1055,20 @@
       <c r="M8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1013,8 +1108,20 @@
       <c r="M9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1054,8 +1161,20 @@
       <c r="M10" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1095,8 +1214,20 @@
       <c r="M11" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1136,8 +1267,20 @@
       <c r="M12" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1177,8 +1320,20 @@
       <c r="M13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" t="s">
+        <v>8</v>
+      </c>
+      <c r="P13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1218,8 +1373,20 @@
       <c r="M14" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1259,8 +1426,20 @@
       <c r="M15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>8</v>
+      </c>
+      <c r="O15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1300,8 +1479,20 @@
       <c r="M16" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1341,8 +1532,20 @@
       <c r="M17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1382,8 +1585,20 @@
       <c r="M18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>8</v>
+      </c>
+      <c r="O18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P18" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1423,8 +1638,20 @@
       <c r="M19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1449,7 +1676,7 @@
       <c r="H20" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="J20" t="s">
@@ -1464,8 +1691,20 @@
       <c r="M20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>9</v>
+      </c>
+      <c r="O20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1490,7 +1729,7 @@
       <c r="H21" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="J21" t="s">
@@ -1505,8 +1744,20 @@
       <c r="M21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1546,8 +1797,20 @@
       <c r="M22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>8</v>
+      </c>
+      <c r="O22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1587,8 +1850,20 @@
       <c r="M23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1634,8 +1909,14 @@
       <c r="O24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1672,8 +1953,20 @@
       <c r="M25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1710,8 +2003,20 @@
       <c r="M26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1749,8 +2054,20 @@
       <c r="M27">
         <v>-20</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>-17</v>
+      </c>
+      <c r="O27">
+        <v>-18</v>
+      </c>
+      <c r="P27">
+        <v>-23</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="C28" s="1"/>
       <c r="E28" s="3"/>
       <c r="H28" s="3"/>

</xml_diff>